<commit_message>
Pbiviz and pbix files latest
</commit_message>
<xml_diff>
--- a/documents/Published/DataInsights/DataInsightsByMAQSoftwareChecklist.xlsx
+++ b/documents/Published/DataInsights/DataInsightsByMAQSoftwareChecklist.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PowerBI\PowerBI-visuals\documents\Published\DataInsights\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PowerBICustomVisuals\documents\Published\DataInsights\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{257AE7EF-0C33-4500-A079-B72777F743DD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{0A959DB4-3E27-42B6-BC52-6DE114CB58CF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1" xr2:uid="{0A959DB4-3E27-42B6-BC52-6DE114CB58CF}"/>
   </bookViews>
   <sheets>
     <sheet name="BVT" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="112">
   <si>
     <t>S no</t>
   </si>
@@ -189,17 +190,39 @@
     <t>Similar for Min, average and constant line</t>
   </si>
   <si>
+    <t>Isolation</t>
+  </si>
+  <si>
     <t>1.Select bar/ Column chart from view as
 2. Go to format pane
 3. Analytics &gt; Toggle on Max Line</t>
   </si>
   <si>
+    <t>1.Select bar/column/ brick chart
+2. click Drag the mouse to select the bars/brick
+3. click on isolate</t>
+  </si>
+  <si>
+    <t>A blue box is drawn on dragging.
+On leaving the mouse the opacity of bars not selected is reduced
+Only the selected bars/bricks are rendered</t>
+  </si>
+  <si>
+    <t>Verify Isolation functionality(Not available for table)</t>
+  </si>
+  <si>
     <t>Reset</t>
   </si>
   <si>
     <t>Verify reset(Reset works only for isolation)</t>
   </si>
   <si>
+    <t>Perform isolation as in 9</t>
+  </si>
+  <si>
+    <t>Click reset. The visual displays all the data</t>
+  </si>
+  <si>
     <t>Undo</t>
   </si>
   <si>
@@ -222,9 +245,6 @@
   </si>
   <si>
     <t>Checklist Point </t>
-  </si>
-  <si>
-    <t>Yes/No </t>
   </si>
   <si>
     <t>Have no console errors in IE 11, Edge, Chrome and Firefox browsers by having query string "unmin = true" in the URL? </t>
@@ -331,12 +351,82 @@
     <t>Top menu bar disappear. Axis labels are present which allows you to change the axis values</t>
   </si>
   <si>
-    <t>1. Click on any bar/column/brick
-2. Click on Reset button</t>
-  </si>
-  <si>
-    <t>The selected bar/brick/column gets higher opacity and others get lower opacity
-Chart is redrawn and opacity gets reset to normal</t>
+    <t>Output After Changes</t>
+  </si>
+  <si>
+    <t>Edge</t>
+  </si>
+  <si>
+    <t>Chrome</t>
+  </si>
+  <si>
+    <t>IE</t>
+  </si>
+  <si>
+    <t>Top Menu bar is present with options
+1. View As
+2. Binning By
+3. X
+4. Y
+5. Color
+6. Text-Color
+7. Color-By(isolate has been removed)</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>Format pane will have:
+1.Legend toggle 
+2.Presentation toggle</t>
+  </si>
+  <si>
+    <t>Format pane will have:
+1.Legend toggle 
+2.Presentation toggle
+3. Analytics &gt;1. MaxLine 2. MinLine 3. Average Line 4. Constant Line
+4. Value dropdown</t>
+  </si>
+  <si>
+    <t>1. Fisrt 2 letters and ellipsis for the value in label is present on the brick in top left corner
+2. Value is present in the bottom right corner
+3. If Binning By is not none then brick for each bin value are present</t>
+  </si>
+  <si>
+    <t>"1. Bar Chart is rendered for every Bin value
+2. Width of bar chat is wrt to Corresponding bin
+"</t>
+  </si>
+  <si>
+    <t>Coloumn selector button is present in the bottom of the visual.
+Top menu display only View as, Binning By, Color, Text color and Color By Button</t>
+  </si>
+  <si>
+    <t>Isolation is removed</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>visual not interactive</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Analytics Option is wrong</t>
+  </si>
+  <si>
+    <t>Show X Axis is wrong</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>Power BI</t>
+  </si>
+  <si>
+    <t>NO(In columnchart)</t>
   </si>
 </sst>
 </file>
@@ -380,7 +470,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -390,6 +480,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -704,10 +795,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD35E9AA-EC94-40B6-87B9-91903B6E03DF}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,10 +806,11 @@
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.28515625" customWidth="1"/>
     <col min="4" max="4" width="36.42578125" customWidth="1"/>
-    <col min="5" max="5" width="67.140625" customWidth="1"/>
+    <col min="5" max="5" width="55.42578125" customWidth="1"/>
+    <col min="6" max="6" width="49.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -734,8 +826,20 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="F1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -751,8 +855,20 @@
       <c r="E2" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="F2" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -768,8 +884,20 @@
       <c r="E3" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="F3" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="H3" t="s">
+        <v>97</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="1" t="s">
@@ -781,8 +909,20 @@
       <c r="E4" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="F4" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="3" t="s">
@@ -794,8 +934,20 @@
       <c r="E5" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="F5" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -811,8 +963,20 @@
       <c r="E6" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="F6" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -828,8 +992,20 @@
       <c r="E7" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="F7" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
@@ -845,8 +1021,20 @@
       <c r="E8" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="F8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
@@ -862,8 +1050,20 @@
       <c r="E9" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="F9" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
@@ -876,8 +1076,20 @@
       <c r="E10" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+      <c r="F10" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8</v>
       </c>
@@ -888,87 +1100,189 @@
         <v>39</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D12" s="3" t="s">
         <v>40</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="F12" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="D13" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="G13" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>87</v>
+        <v>50</v>
       </c>
       <c r="E15" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D17" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" t="s">
+        <v>57</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>12</v>
+      </c>
+      <c r="B18" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>10</v>
-      </c>
-      <c r="B16" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D17" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>11</v>
-      </c>
-      <c r="B18" t="s">
-        <v>83</v>
-      </c>
       <c r="C18" s="3" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>86</v>
+        <v>91</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -977,274 +1291,489 @@
     <mergeCell ref="B3:B5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA835CA9-E288-452C-87F2-A429070D6D1E}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" customWidth="1"/>
-    <col min="2" max="2" width="90.85546875" customWidth="1"/>
+    <col min="2" max="2" width="152.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.5703125" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B1" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="C7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="C8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="C9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="C10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C15" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="C16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>72</v>
-      </c>
-      <c r="C17" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="C18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="C19" t="s">
+        <v>106</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="C20" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="C21" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+      <c r="C23" t="s">
+        <v>107</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>108</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>19</v>
       </c>
       <c r="B26" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C26" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>20</v>
       </c>
       <c r="B27" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C27" t="s">
-        <v>59</v>
+        <v>109</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Issues of brick chart and bar chart fixed for header and selection/deselection
</commit_message>
<xml_diff>
--- a/documents/Published/DataInsights/DataInsightsByMAQSoftwareChecklist.xlsx
+++ b/documents/Published/DataInsights/DataInsightsByMAQSoftwareChecklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PowerBICustomVisuals\documents\Published\DataInsights\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cutom Visual\PowerBI\documents\Published\DataInsights\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{257AE7EF-0C33-4500-A079-B72777F743DD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8A4538-1ABB-4AB5-BC91-F7FB51CD66BB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1" xr2:uid="{0A959DB4-3E27-42B6-BC52-6DE114CB58CF}"/>
   </bookViews>
@@ -46,16 +46,6 @@
     <t xml:space="preserve"> -</t>
   </si>
   <si>
-    <t>Top Menu bar is present with options
-1. View As
-2. Binning By
-3. X
-4. Y
-5. Color
-6. Text-Color
-7. Isolate</t>
-  </si>
-  <si>
     <t>Render visual for first time</t>
   </si>
   <si>
@@ -388,11 +378,6 @@
 4. Value dropdown</t>
   </si>
   <si>
-    <t>1. Fisrt 2 letters and ellipsis for the value in label is present on the brick in top left corner
-2. Value is present in the bottom right corner
-3. If Binning By is not none then brick for each bin value are present</t>
-  </si>
-  <si>
     <t>"1. Bar Chart is rendered for every Bin value
 2. Width of bar chat is wrt to Corresponding bin
 "</t>
@@ -427,6 +412,20 @@
   </si>
   <si>
     <t>NO(In columnchart)</t>
+  </si>
+  <si>
+    <t>Top Menu bar is present with options
+1. View As
+2. Binning By
+3. X
+4. Y
+5. Color
+6. Text-Color</t>
+  </si>
+  <si>
+    <t>1. Now Brick header is same as the brick width
+2. Value is present in the bottom right corner
+3. If Binning By is not none then brick for each bin value are present</t>
   </si>
 </sst>
 </file>
@@ -477,10 +476,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -797,8 +796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD35E9AA-EC94-40B6-87B9-91903B6E03DF}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -827,16 +826,16 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="120" x14ac:dyDescent="0.25">
@@ -847,104 +846,104 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="G2" s="3" t="s">
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="G3" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="H3" t="s">
+        <v>96</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="D5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="H3" t="s">
-        <v>97</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>99</v>
-      </c>
       <c r="G5" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="105" x14ac:dyDescent="0.25">
@@ -952,28 +951,28 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="D6" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="120" x14ac:dyDescent="0.25">
@@ -981,28 +980,28 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="D7" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="105" x14ac:dyDescent="0.25">
@@ -1010,28 +1009,28 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="D8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>30</v>
-      </c>
       <c r="F8" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -1039,28 +1038,28 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="F9" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -1068,25 +1067,25 @@
         <v>7</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="E10" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="F10" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="165" x14ac:dyDescent="0.25">
@@ -1094,62 +1093,62 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="D11" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="F12" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="D13" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -1157,28 +1156,28 @@
         <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D14" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="F14" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1186,25 +1185,25 @@
         <v>10</v>
       </c>
       <c r="B15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="E15" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>51</v>
-      </c>
       <c r="G15" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1212,48 +1211,48 @@
         <v>11</v>
       </c>
       <c r="B16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="E16" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="F16" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D17" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>57</v>
-      </c>
       <c r="F17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1261,28 +1260,28 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="D18" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="E18" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>91</v>
-      </c>
       <c r="F18" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1300,7 +1299,7 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1314,22 +1313,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" t="s">
         <v>58</v>
       </c>
-      <c r="B1" t="s">
-        <v>59</v>
-      </c>
       <c r="C1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>93</v>
+        <v>108</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1337,19 +1336,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1357,19 +1356,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>109</v>
+        <v>60</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1377,19 +1376,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>111</v>
+        <v>102</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1397,37 +1396,37 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F5" s="5"/>
+        <v>60</v>
+      </c>
+      <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1435,69 +1434,69 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F7" s="5"/>
+        <v>60</v>
+      </c>
+      <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="5"/>
+      <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F9" s="5"/>
+        <v>60</v>
+      </c>
+      <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1505,19 +1504,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1525,48 +1524,48 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F12" s="5"/>
+        <v>60</v>
+      </c>
+      <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="5"/>
+      <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C14" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1574,19 +1573,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>109</v>
+        <v>102</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1594,19 +1593,19 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>104</v>
+        <v>60</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1614,42 +1613,42 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="5" t="s">
-        <v>104</v>
+      <c r="F17" s="4" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E18" s="1"/>
-      <c r="F18" s="5" t="s">
-        <v>104</v>
+      <c r="F18" s="4" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C19" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E19" s="1"/>
-      <c r="F19" s="5" t="s">
-        <v>109</v>
+      <c r="F19" s="4" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1657,99 +1656,99 @@
         <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F20" s="5"/>
+        <v>60</v>
+      </c>
+      <c r="F20" s="4"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C21" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="5"/>
+      <c r="F22" s="4"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C23" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F23" s="5"/>
+        <v>105</v>
+      </c>
+      <c r="F23" s="4"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="5"/>
+      <c r="F25" s="4"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>19</v>
       </c>
       <c r="B26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C26" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1757,19 +1756,19 @@
         <v>20</v>
       </c>
       <c r="B27" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C27" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>104</v>
+        <v>107</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Bar Multiple Selection/Deselection Feature
</commit_message>
<xml_diff>
--- a/documents/Published/DataInsights/DataInsightsByMAQSoftwareChecklist.xlsx
+++ b/documents/Published/DataInsights/DataInsightsByMAQSoftwareChecklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cutom Visual\PowerBI\documents\Published\DataInsights\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8A4538-1ABB-4AB5-BC91-F7FB51CD66BB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64D02AF8-FC70-4EF8-85D2-33DFFF0821AD}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1" xr2:uid="{0A959DB4-3E27-42B6-BC52-6DE114CB58CF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{0A959DB4-3E27-42B6-BC52-6DE114CB58CF}"/>
   </bookViews>
   <sheets>
     <sheet name="BVT" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="111">
   <si>
     <t>S no</t>
   </si>
@@ -378,11 +378,6 @@
 4. Value dropdown</t>
   </si>
   <si>
-    <t>"1. Bar Chart is rendered for every Bin value
-2. Width of bar chat is wrt to Corresponding bin
-"</t>
-  </si>
-  <si>
     <t>Coloumn selector button is present in the bottom of the visual.
 Top menu display only View as, Binning By, Color, Text color and Color By Button</t>
   </si>
@@ -425,7 +420,8 @@
   <si>
     <t>1. Now Brick header is same as the brick width
 2. Value is present in the bottom right corner
-3. If Binning By is not none then brick for each bin value are present</t>
+3. If Binning By is not none then brick for each bin value are present
+4. Multiple Bar Selection/Deselection Holding Ctrl button</t>
   </si>
 </sst>
 </file>
@@ -796,8 +792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD35E9AA-EC94-40B6-87B9-91903B6E03DF}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -852,7 +848,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>95</v>
@@ -963,7 +959,7 @@
         <v>22</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>96</v>
@@ -992,7 +988,7 @@
         <v>23</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>99</v>
+        <v>23</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>96</v>
@@ -1050,7 +1046,7 @@
         <v>33</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>96</v>
@@ -1168,7 +1164,7 @@
         <v>45</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>63</v>
@@ -1298,7 +1294,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA835CA9-E288-452C-87F2-A429070D6D1E}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
@@ -1325,7 +1321,7 @@
         <v>93</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>92</v>
@@ -1339,16 +1335,16 @@
         <v>59</v>
       </c>
       <c r="C2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1368,7 +1364,7 @@
         <v>60</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1379,16 +1375,16 @@
         <v>62</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1417,16 +1413,16 @@
         <v>65</v>
       </c>
       <c r="C6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1437,10 +1433,10 @@
         <v>66</v>
       </c>
       <c r="C7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>60</v>
@@ -1487,16 +1483,16 @@
         <v>69</v>
       </c>
       <c r="C10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1507,16 +1503,16 @@
         <v>70</v>
       </c>
       <c r="C11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1556,16 +1552,16 @@
         <v>73</v>
       </c>
       <c r="C14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1576,16 +1572,16 @@
         <v>74</v>
       </c>
       <c r="C15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1605,7 +1601,7 @@
         <v>60</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1618,7 +1614,7 @@
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1633,7 +1629,7 @@
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1641,14 +1637,14 @@
         <v>78</v>
       </c>
       <c r="C19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1677,16 +1673,16 @@
         <v>80</v>
       </c>
       <c r="C21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1702,25 +1698,25 @@
         <v>82</v>
       </c>
       <c r="C23" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F23" s="4"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1739,16 +1735,16 @@
         <v>84</v>
       </c>
       <c r="C26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1759,16 +1755,16 @@
         <v>85</v>
       </c>
       <c r="C27" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>